<commit_message>
Addressed Issue #s 27,28
</commit_message>
<xml_diff>
--- a/Draft Schema/Draft Animal Health and Treatments.xlsx
+++ b/Draft Schema/Draft Animal Health and Treatments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagaraja\Dropbox (Rezare Systems)\RezareProjects\MLA\ISC Animal Schema\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094A7261-CB09-4A6E-9E4C-B45683C02F2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BEFBAA-E487-445C-A070-DC38FC5857A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="7">iscDoseType!$A$1:$G$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">iscMedicineResource!$A$1:$G$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">iscTreatmentEvent!$A$1:$G$43</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">iscTreatmentProgrammeEvent!$A$1:$G$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">iscTreatmentProgrammeEvent!$A$1:$G$38</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="8">iscWithdrawalType!$A$1:$G$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +42,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="143">
   <si>
     <t>Entity</t>
   </si>
@@ -192,9 +194,6 @@
     <t>Name of the medicine or remedy given for this treatment</t>
   </si>
   <si>
-    <t>An indicatorr whether the medicine or remedy is an approved medicine</t>
-  </si>
-  <si>
     <t>enum (Y,N)</t>
   </si>
   <si>
@@ -252,16 +251,10 @@
     <t>iscDose</t>
   </si>
   <si>
-    <t>Date of administration of dose</t>
-  </si>
-  <si>
     <t>doseQuantity</t>
   </si>
   <si>
     <t>doseUnits</t>
-  </si>
-  <si>
-    <t>administeredBy</t>
   </si>
   <si>
     <t>reasonForAdministraton</t>
@@ -313,15 +306,9 @@
     <t>Details of medicine dose administered</t>
   </si>
   <si>
-    <t>Name of the person administering the treatment</t>
-  </si>
-  <si>
     <t>Quantity of dose administered</t>
   </si>
   <si>
-    <t>Units of measurement in which the dose was measured and administered</t>
-  </si>
-  <si>
     <t>This attribute can be used to when medicine has been administered without a diagnosis</t>
   </si>
   <si>
@@ -359,9 +346,6 @@
   </si>
   <si>
     <t>Cephalosporin</t>
-  </si>
-  <si>
-    <t>2017-12-28</t>
   </si>
   <si>
     <t>1.5</t>
@@ -457,6 +441,52 @@
   </si>
   <si>
     <t>Animal Health and Treatments</t>
+  </si>
+  <si>
+    <t>responsible</t>
+  </si>
+  <si>
+    <t>Person responsible for the treatment programme</t>
+  </si>
+  <si>
+    <t>Person responsible for the diagnosis</t>
+  </si>
+  <si>
+    <t>Person responsible for the treatment</t>
+  </si>
+  <si>
+    <t>enum</t>
+  </si>
+  <si>
+    <t>Enum ( 'Plan', 'Actual')</t>
+  </si>
+  <si>
+    <t>planOrActual</t>
+  </si>
+  <si>
+    <t>Indicator showing if the attributes in the course Summary are actual information for the  treatments or the plan</t>
+  </si>
+  <si>
+    <t>uncefactMassUnits.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Units of measurement in which the dose was measured and administered as specified in UN/CEFACT 3-letter form. Useful unts for dose could be MLT(millilitres),LTR(litres),MGM(milligrams),GRM(grams),XTU( tube -X prefix as its an ISO 21 packaging unit, as per the ISO 20 recommendation),XVI (vial -X prefix as above),XAR (suppository -X prefix as above),XCQ(cartridge -X prefix as above),GJ(gram per millilitre)GL(gram per litre),GRN(grain),L19(millilitre per litre),NA(milligram per kilogram),SYR(syringe),VP(percent volume),WW(volume equal to millilitres of water)
+</t>
+  </si>
+  <si>
+    <t>batches</t>
+  </si>
+  <si>
+    <t>array of batch information</t>
+  </si>
+  <si>
+    <t>Batches and expiry details of the medicine administered</t>
+  </si>
+  <si>
+    <t>An indicator whether the medicine or remedy is an approved medicine</t>
+  </si>
+  <si>
+    <t>array of Batch information</t>
   </si>
 </sst>
 </file>
@@ -800,6 +830,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -809,7 +840,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
@@ -1161,7 +1191,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,34 +1208,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
-        <v>133</v>
+      <c r="A1" s="66" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="3" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
     </row>
     <row r="4" spans="1:8" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26"/>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
     </row>
@@ -1568,10 +1598,10 @@
     <tabColor theme="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,29 +1618,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
     </row>
@@ -1667,62 +1697,67 @@
       <c r="B7" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>79</v>
+      <c r="C7" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="39"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="G7" s="53"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="64" t="s">
-        <v>105</v>
-      </c>
+      <c r="A8" s="54"/>
       <c r="B8" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1" t="s">
-        <v>80</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="53"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="64" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="64" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="F10" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>8</v>
-      </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="28"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>9</v>
       </c>
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
@@ -1731,7 +1766,9 @@
       <c r="F12" s="28"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+      <c r="A13" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="B13" s="27"/>
       <c r="C13" s="27"/>
       <c r="D13" s="12"/>
@@ -1739,9 +1776,7 @@
       <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>10</v>
-      </c>
+      <c r="A14" s="22"/>
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
       <c r="D14" s="12"/>
@@ -1749,64 +1784,66 @@
       <c r="F14" s="28"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="11" t="s">
+        <v>10</v>
+      </c>
       <c r="B15" s="27"/>
-      <c r="D15" s="4"/>
-      <c r="F15" s="8"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="28"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="27"/>
       <c r="D16" s="4"/>
-      <c r="F16" s="7"/>
+      <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="F17" s="8"/>
+      <c r="D17" s="4"/>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="D18" s="4"/>
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="10"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="D21" s="17"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="20"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="28"/>
       <c r="G21" s="18"/>
-      <c r="H21" s="22"/>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="14"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="19"/>
       <c r="F22" s="20"/>
       <c r="G22" s="18"/>
       <c r="H22" s="22"/>
     </row>
     <row r="23" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
-      <c r="D23" s="17"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="14"/>
-      <c r="F23" s="28"/>
+      <c r="F23" s="20"/>
       <c r="G23" s="18"/>
       <c r="H23" s="22"/>
     </row>
     <row r="24" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
-      <c r="D24" s="12"/>
+      <c r="D24" s="17"/>
       <c r="E24" s="14"/>
       <c r="F24" s="28"/>
       <c r="G24" s="18"/>
@@ -1815,7 +1852,7 @@
     <row r="25" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="D25" s="12"/>
-      <c r="E25" s="23"/>
+      <c r="E25" s="14"/>
       <c r="F25" s="28"/>
       <c r="G25" s="18"/>
       <c r="H25" s="22"/>
@@ -1823,30 +1860,30 @@
     <row r="26" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="24"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="28"/>
       <c r="G26" s="18"/>
       <c r="H26" s="22"/>
     </row>
     <row r="27" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="D27" s="12"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="28"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="18"/>
       <c r="H27" s="22"/>
     </row>
     <row r="28" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="D28" s="12"/>
-      <c r="E28" s="14"/>
+      <c r="E28" s="21"/>
       <c r="F28" s="28"/>
-      <c r="G28" s="18"/>
       <c r="H28" s="22"/>
     </row>
     <row r="29" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="D29" s="12"/>
-      <c r="E29" s="19"/>
+      <c r="E29" s="14"/>
       <c r="F29" s="28"/>
       <c r="G29" s="18"/>
       <c r="H29" s="22"/>
@@ -1854,7 +1891,7 @@
     <row r="30" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="D30" s="12"/>
-      <c r="E30" s="14"/>
+      <c r="E30" s="19"/>
       <c r="F30" s="28"/>
       <c r="G30" s="18"/>
       <c r="H30" s="22"/>
@@ -1870,9 +1907,9 @@
     <row r="32" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
+      <c r="E32" s="14"/>
       <c r="F32" s="28"/>
-      <c r="G32" s="12"/>
+      <c r="G32" s="18"/>
       <c r="H32" s="22"/>
     </row>
     <row r="33" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -1909,58 +1946,66 @@
     </row>
     <row r="37" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="14"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
       <c r="F37" s="28"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="22"/>
     </row>
     <row r="38" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
-      <c r="D38" s="12"/>
+      <c r="D38" s="17"/>
       <c r="E38" s="14"/>
       <c r="F38" s="28"/>
     </row>
     <row r="39" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="1"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="28"/>
     </row>
     <row r="40" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="28"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="27"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="32"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="14"/>
       <c r="F41" s="28"/>
-      <c r="G41" s="29"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" s="27"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="8"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="29"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="28"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="8"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B44" s="27"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="8"/>
-      <c r="H44" s="28"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="28"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="27"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="8"/>
+      <c r="H45" s="28"/>
     </row>
   </sheetData>
   <dataConsolidate>
@@ -1984,10 +2029,10 @@
     <tabColor theme="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2004,29 +2049,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
-        <v>125</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="A1" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
       <c r="F2" s="57"/>
       <c r="G2" s="57"/>
     </row>
     <row r="3" spans="1:7" s="55" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="57"/>
       <c r="G3" s="57"/>
     </row>
@@ -2063,7 +2108,7 @@
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B6" s="51" t="s">
         <v>32</v>
@@ -2079,46 +2124,51 @@
       <c r="G6" s="53"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
       <c r="B7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="53"/>
+        <v>128</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="39"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="54"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="54"/>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="56"/>
+      <c r="A10" s="54"/>
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="56"/>
       <c r="F11" s="28"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
@@ -2127,7 +2177,9 @@
       <c r="F12" s="28"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+      <c r="A13" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="B13" s="27"/>
       <c r="C13" s="27"/>
       <c r="D13" s="12"/>
@@ -2135,9 +2187,7 @@
       <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>10</v>
-      </c>
+      <c r="A14" s="22"/>
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
       <c r="D14" s="12"/>
@@ -2145,23 +2195,28 @@
       <c r="F14" s="28"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="11" t="s">
+        <v>10</v>
+      </c>
       <c r="B15" s="27"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="27"/>
       <c r="D16" s="4"/>
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
+      <c r="D17" s="4"/>
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="D18" s="4"/>
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2169,9 +2224,11 @@
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="14"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="33"/>
       <c r="F20" s="28"/>
       <c r="G20" s="18"/>
       <c r="H20" s="55"/>
@@ -2179,22 +2236,22 @@
     <row r="21" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="D21" s="17"/>
-      <c r="E21" s="19"/>
+      <c r="E21" s="14"/>
       <c r="F21" s="20"/>
       <c r="G21" s="18"/>
       <c r="H21" s="22"/>
     </row>
     <row r="22" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="14"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="19"/>
       <c r="F22" s="20"/>
       <c r="G22" s="18"/>
       <c r="H22" s="22"/>
     </row>
     <row r="23" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
-      <c r="D23" s="17"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="14"/>
       <c r="F23" s="28"/>
       <c r="G23" s="18"/>
@@ -2202,7 +2259,7 @@
     </row>
     <row r="24" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
-      <c r="D24" s="12"/>
+      <c r="D24" s="17"/>
       <c r="E24" s="14"/>
       <c r="F24" s="28"/>
       <c r="G24" s="18"/>
@@ -2211,7 +2268,7 @@
     <row r="25" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="D25" s="12"/>
-      <c r="E25" s="23"/>
+      <c r="E25" s="14"/>
       <c r="F25" s="28"/>
       <c r="G25" s="18"/>
       <c r="H25" s="22"/>
@@ -2219,7 +2276,7 @@
     <row r="26" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="14"/>
+      <c r="E26" s="23"/>
       <c r="F26" s="24"/>
       <c r="G26" s="18"/>
       <c r="H26" s="22"/>
@@ -2227,14 +2284,14 @@
     <row r="27" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="D27" s="12"/>
-      <c r="E27" s="56"/>
+      <c r="E27" s="14"/>
       <c r="F27" s="28"/>
       <c r="H27" s="22"/>
     </row>
     <row r="28" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="D28" s="12"/>
-      <c r="E28" s="14"/>
+      <c r="E28" s="56"/>
       <c r="F28" s="28"/>
       <c r="G28" s="18"/>
       <c r="H28" s="22"/>
@@ -2242,7 +2299,7 @@
     <row r="29" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="D29" s="12"/>
-      <c r="E29" s="19"/>
+      <c r="E29" s="14"/>
       <c r="F29" s="28"/>
       <c r="G29" s="18"/>
       <c r="H29" s="22"/>
@@ -2250,7 +2307,7 @@
     <row r="30" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="D30" s="12"/>
-      <c r="E30" s="14"/>
+      <c r="E30" s="19"/>
       <c r="F30" s="28"/>
       <c r="G30" s="18"/>
       <c r="H30" s="22"/>
@@ -2266,7 +2323,7 @@
     <row r="32" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
+      <c r="E32" s="14"/>
       <c r="F32" s="28"/>
       <c r="G32" s="12"/>
       <c r="H32" s="22"/>
@@ -2305,58 +2362,65 @@
     </row>
     <row r="37" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="14"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
       <c r="F37" s="28"/>
     </row>
     <row r="38" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
-      <c r="D38" s="12"/>
+      <c r="D38" s="17"/>
       <c r="E38" s="14"/>
       <c r="F38" s="28"/>
     </row>
     <row r="39" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="33"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="14"/>
       <c r="F39" s="8"/>
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="14"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="33"/>
       <c r="F40" s="28"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
       <c r="B41" s="27"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="32"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="14"/>
       <c r="F41" s="28"/>
       <c r="G41" s="29"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" s="27"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="35"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="32"/>
       <c r="F42" s="8"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="14"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="35"/>
       <c r="F43" s="28"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B44" s="27"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="56"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="14"/>
       <c r="F44" s="8"/>
       <c r="H44" s="28"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="27"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="56"/>
     </row>
   </sheetData>
   <dataConsolidate>
@@ -2400,29 +2464,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
     </row>
@@ -2478,10 +2542,10 @@
       </c>
       <c r="D7" s="39"/>
       <c r="E7" s="40" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F7" s="39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2494,58 +2558,58 @@
       </c>
       <c r="D8" s="39"/>
       <c r="E8" s="40" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F8" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="39" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="39"/>
       <c r="E9" s="40" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F9" s="39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="62" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="39"/>
       <c r="E10" s="52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F10" s="58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="39" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C11" s="39" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="39"/>
       <c r="E11" s="40" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F11" s="39" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2838,7 +2902,7 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2855,31 +2919,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="A1" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="67" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
+      <c r="B2" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
       <c r="F2" s="57"/>
       <c r="G2" s="57"/>
     </row>
     <row r="3" spans="1:7" s="55" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="57"/>
       <c r="G3" s="57"/>
     </row>
@@ -2916,7 +2980,7 @@
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
@@ -2926,111 +2990,117 @@
       <c r="G6" s="53"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>77</v>
-      </c>
+      <c r="A7" s="54"/>
+      <c r="B7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="61">
+        <v>43094</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="53"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="39" t="s">
-        <v>90</v>
-      </c>
+      <c r="A8" s="54"/>
+      <c r="B8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="61">
+        <v>43099</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="53"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="39" t="s">
-        <v>117</v>
+        <v>39</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="D9" s="39"/>
-      <c r="E9" s="40" t="s">
-        <v>119</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>118</v>
+      <c r="E9" s="40"/>
+      <c r="F9" s="39" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="39" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="C10" s="39" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="39"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="39" t="s">
-        <v>89</v>
+      <c r="E10" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E11" s="61">
-        <v>43094</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="B11" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="39"/>
+      <c r="E11" s="40" t="s">
         <v>91</v>
       </c>
+      <c r="F11" s="28" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="61">
-        <v>43099</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>92</v>
+      <c r="A12" s="3"/>
+      <c r="B12" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="39"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="39" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>138</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>139</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>49</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3041,33 +3111,41 @@
         <v>7</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="33" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="59"/>
-      <c r="C17" s="1"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="60" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="8"/>
+      <c r="E17" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="27"/>
@@ -3337,7 +3415,7 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3354,29 +3432,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="A1" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
     </row>
@@ -3405,7 +3483,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="51" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -3415,7 +3493,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
@@ -3432,7 +3510,7 @@
         <v>39</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D7" s="39"/>
       <c r="E7" s="52"/>
@@ -3442,24 +3520,27 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="51"/>
       <c r="B8" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="65" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="F9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3470,81 +3551,81 @@
         <v>7</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="59" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="60" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="21"/>
       <c r="F13" s="28" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="56" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="1" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="56" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
@@ -3844,7 +3925,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3861,29 +3942,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
     </row>
@@ -3949,7 +4030,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>45</v>
@@ -3963,10 +4044,10 @@
         <v>7</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>46</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3977,7 +4058,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -4272,7 +4353,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4289,29 +4370,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="A1" s="67" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
       <c r="F2" s="57"/>
       <c r="G2" s="57"/>
     </row>
     <row r="3" spans="1:7" s="55" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="57"/>
       <c r="G3" s="57"/>
     </row>
@@ -4348,7 +4429,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
@@ -4359,45 +4440,34 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="51"/>
-      <c r="B7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>136</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>88</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4709,29 +4779,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="A1" s="67" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
       <c r="F2" s="57"/>
       <c r="G2" s="57"/>
     </row>
     <row r="3" spans="1:7" s="55" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="57"/>
       <c r="G3" s="57"/>
     </row>
@@ -4768,7 +4838,7 @@
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
@@ -4780,33 +4850,33 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="39" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C7" s="39" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="39"/>
       <c r="E7" s="40" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F7" s="39" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="39" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D8" s="39"/>
       <c r="E8" s="40" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F8" s="39" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated changes to Medicine Resource
</commit_message>
<xml_diff>
--- a/Draft Schema/Draft Animal Health and Treatments.xlsx
+++ b/Draft Schema/Draft Animal Health and Treatments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagaraja\Dropbox (Rezare Systems)\RezareProjects\MLA\ISC Animal Schema\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112F8DA4-5044-4904-A7E4-ECC28020AFF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC86DE58-BFB3-4656-8BBA-6F25D6C3F13D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="749" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="749" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="icarEventCoreResource" sheetId="14" r:id="rId1"/>
@@ -19,20 +19,22 @@
     <sheet name="iscDiagnosisType" sheetId="34" r:id="rId4"/>
     <sheet name="iscCourseSummaryType" sheetId="43" r:id="rId5"/>
     <sheet name="iscTreatmentEvent" sheetId="25" r:id="rId6"/>
-    <sheet name="iscMedicineResource" sheetId="39" r:id="rId7"/>
-    <sheet name="iscDoseType" sheetId="44" r:id="rId8"/>
-    <sheet name="iscWithdrawalType" sheetId="45" r:id="rId9"/>
+    <sheet name="iscMedicineRefType" sheetId="47" r:id="rId7"/>
+    <sheet name="iscMedicineResource" sheetId="39" r:id="rId8"/>
+    <sheet name="iscDoseType" sheetId="44" r:id="rId9"/>
+    <sheet name="iscWithdrawalType" sheetId="45" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">icarEventCoreResource!$A$2:$G$31</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">iscCourseSummaryType!$A$1:$G$43</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">iscDiagnosisEventResource!$A$1:$G$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">iscDiagnosisType!$A$1:$G$41</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">iscDoseType!$A$1:$G$37</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">iscMedicineResource!$A$1:$G$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">iscDoseType!$A$1:$G$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">iscMedicineRefType!$A$1:$G$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">iscMedicineResource!$A$1:$G$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">iscTreatmentEvent!$A$1:$G$43</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">iscTreatmentProgrammeEvent!$A$1:$G$38</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="8">iscWithdrawalType!$A$1:$G$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="9">iscWithdrawalType!$A$1:$G$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="147">
   <si>
     <t>Entity</t>
   </si>
@@ -179,9 +181,6 @@
     <t>batch</t>
   </si>
   <si>
-    <t>iscMedicine</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -496,6 +495,12 @@
   </si>
   <si>
     <t>Indicates the market the withdrawal applies to</t>
+  </si>
+  <si>
+    <t>iscMedicineREsource inherits allOf icarResource</t>
+  </si>
+  <si>
+    <t>iscMedicineRefType</t>
   </si>
 </sst>
 </file>
@@ -1218,7 +1223,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="66" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -1601,6 +1606,421 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B0327C-9953-4813-9573-3D0583D807FE}">
+  <sheetPr>
+    <tabColor theme="0"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H47"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="46.5703125" style="33" customWidth="1"/>
+    <col min="6" max="6" width="99.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="41.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+    </row>
+    <row r="2" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+    </row>
+    <row r="3" spans="1:7" s="55" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+    </row>
+    <row r="4" spans="1:7" s="11" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="53"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="39"/>
+      <c r="E7" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="39"/>
+      <c r="E8" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="39"/>
+      <c r="E9" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="14" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="28"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="28"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="28"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="28"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="27"/>
+      <c r="D18" s="4"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="D21" s="4"/>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="55"/>
+    </row>
+    <row r="24" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="22"/>
+    </row>
+    <row r="25" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="22"/>
+    </row>
+    <row r="26" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="22"/>
+    </row>
+    <row r="27" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="22"/>
+    </row>
+    <row r="28" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="22"/>
+    </row>
+    <row r="29" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="22"/>
+    </row>
+    <row r="30" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="28"/>
+      <c r="H30" s="22"/>
+    </row>
+    <row r="31" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="22"/>
+    </row>
+    <row r="32" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="22"/>
+    </row>
+    <row r="33" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="22"/>
+    </row>
+    <row r="34" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="22"/>
+    </row>
+    <row r="35" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="22"/>
+    </row>
+    <row r="36" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="22"/>
+    </row>
+    <row r="37" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="22"/>
+    </row>
+    <row r="38" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="22"/>
+    </row>
+    <row r="39" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="22"/>
+    </row>
+    <row r="40" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="28"/>
+    </row>
+    <row r="41" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="28"/>
+    </row>
+    <row r="42" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="28"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="27"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="29"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="27"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="28"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="27"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="8"/>
+      <c r="H47" s="28"/>
+    </row>
+  </sheetData>
+  <dataConsolidate>
+    <dataRefs count="1">
+      <dataRef ref="A2:H2" sheet="Status" r:id="rId1"/>
+    </dataRefs>
+  </dataConsolidate>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{522F9608-03C5-4846-91FA-14CB354CF4BC}">
   <sheetPr>
@@ -1610,7 +2030,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1704,7 +2124,7 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="54"/>
       <c r="B7" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C7" s="39" t="s">
         <v>7</v>
@@ -1712,46 +2132,46 @@
       <c r="D7" s="39"/>
       <c r="E7" s="52"/>
       <c r="F7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G7" s="53"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="54"/>
       <c r="B8" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G8" s="53"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="64"/>
       <c r="B9" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="64"/>
       <c r="B10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2055,7 +2475,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -2113,7 +2533,7 @@
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="51" t="s">
         <v>32</v>
@@ -2130,7 +2550,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C7" s="39" t="s">
         <v>7</v>
@@ -2138,7 +2558,7 @@
       <c r="D7" s="39"/>
       <c r="E7" s="52"/>
       <c r="F7" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -2148,10 +2568,10 @@
         <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2547,72 +2967,72 @@
       </c>
       <c r="D7" s="39"/>
       <c r="E7" s="40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F7" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="39" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="39"/>
       <c r="E8" s="40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F8" s="39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="39" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="39"/>
       <c r="E9" s="40" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F9" s="39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="62" t="s">
         <v>138</v>
-      </c>
-      <c r="C10" s="62" t="s">
-        <v>139</v>
       </c>
       <c r="D10" s="39"/>
       <c r="E10" s="52"/>
       <c r="F10" s="58" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" s="39" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="39"/>
       <c r="E11" s="40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F11" s="39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2923,7 +3343,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -2933,7 +3353,7 @@
     <row r="2" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
       <c r="B2" s="68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="68"/>
       <c r="D2" s="68"/>
@@ -2983,7 +3403,7 @@
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
@@ -2995,32 +3415,32 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="54"/>
       <c r="B7" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" s="61">
         <v>43094</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G7" s="53"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="54"/>
       <c r="B8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" s="61">
         <v>43099</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G8" s="53"/>
     </row>
@@ -3030,50 +3450,50 @@
         <v>39</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D9" s="39"/>
       <c r="E9" s="40"/>
       <c r="F9" s="39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" s="39" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="39"/>
       <c r="E10" s="40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" s="39" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="39"/>
       <c r="E11" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="39" t="s">
         <v>7</v>
@@ -3081,29 +3501,29 @@
       <c r="D12" s="39"/>
       <c r="E12" s="40"/>
       <c r="F12" s="39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="F13" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3114,40 +3534,40 @@
         <v>7</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -3418,7 +3838,7 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3436,7 +3856,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -3486,7 +3906,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -3496,7 +3916,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
@@ -3513,28 +3933,28 @@
         <v>39</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>94</v>
+        <v>146</v>
       </c>
       <c r="D7" s="39"/>
       <c r="E7" s="52"/>
       <c r="F7" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G7" s="53"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="51"/>
       <c r="B8" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="65" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -3542,10 +3962,10 @@
         <v>40</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3556,81 +3976,81 @@
         <v>7</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="59" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="F12" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="21"/>
       <c r="F13" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="56" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
@@ -3922,7 +4342,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538625A2-C1E4-478E-9220-480EA02404B5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1310FF73-DD05-4023-B42E-67E60815034E}">
   <sheetPr>
     <tabColor theme="0"/>
     <pageSetUpPr fitToPage="1"/>
@@ -3930,7 +4350,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3948,30 +4368,30 @@
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>41</v>
+        <v>146</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
       <c r="D1" s="67"/>
       <c r="E1" s="67"/>
     </row>
-    <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
       <c r="B2" s="68"/>
       <c r="C2" s="68"/>
       <c r="D2" s="68"/>
       <c r="E2" s="68"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-    </row>
-    <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+    </row>
+    <row r="3" spans="1:7" s="55" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
       <c r="B3" s="69"/>
       <c r="C3" s="69"/>
       <c r="D3" s="69"/>
       <c r="E3" s="69"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
     </row>
     <row r="4" spans="1:7" s="11" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
@@ -4006,7 +4426,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
-        <v>41</v>
+        <v>146</v>
       </c>
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
@@ -4029,44 +4449,44 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="21"/>
+      <c r="E10" s="56"/>
       <c r="F10" s="55" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
@@ -4141,7 +4561,7 @@
       <c r="E20" s="33"/>
       <c r="F20" s="28"/>
       <c r="G20" s="18"/>
-      <c r="H20" s="10"/>
+      <c r="H20" s="55"/>
     </row>
     <row r="21" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
@@ -4201,7 +4621,7 @@
     <row r="28" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="D28" s="12"/>
-      <c r="E28" s="21"/>
+      <c r="E28" s="56"/>
       <c r="F28" s="28"/>
       <c r="G28" s="18"/>
       <c r="H28" s="22"/>
@@ -4330,7 +4750,7 @@
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" s="27"/>
       <c r="D45" s="4"/>
-      <c r="E45" s="21"/>
+      <c r="E45" s="56"/>
     </row>
   </sheetData>
   <dataConsolidate>
@@ -4344,7 +4764,7 @@
     <mergeCell ref="B3:E3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F7" r:id="rId2" display="https://github.com/adewg/ICAR/blob/master/Release Candidate Messages/icarResourceReferenceType.json" xr:uid="{0560007B-2D8F-444D-8CE6-B8B4110E7BF3}"/>
+    <hyperlink ref="F7" r:id="rId2" display="https://github.com/adewg/ICAR/blob/master/Release Candidate Messages/icarResourceReferenceType.json" xr:uid="{DB9E105E-FEC8-431F-9B88-74FBC7ADDE86}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape" r:id="rId3"/>
@@ -4352,6 +4772,425 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538625A2-C1E4-478E-9220-480EA02404B5}">
+  <sheetPr>
+    <tabColor theme="0"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" style="33" customWidth="1"/>
+    <col min="6" max="6" width="99.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="41.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+    </row>
+    <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="1:7" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+    </row>
+    <row r="4" spans="1:7" s="11" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="51" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="53"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="51"/>
+      <c r="F7" s="36"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="55" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="56"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="28"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="28"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="28"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="27"/>
+      <c r="D16" s="4"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="10"/>
+    </row>
+    <row r="21" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="22"/>
+    </row>
+    <row r="22" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="22"/>
+    </row>
+    <row r="23" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="22"/>
+    </row>
+    <row r="24" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="22"/>
+    </row>
+    <row r="25" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="22"/>
+    </row>
+    <row r="26" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="22"/>
+    </row>
+    <row r="27" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="28"/>
+      <c r="H27" s="22"/>
+    </row>
+    <row r="28" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="22"/>
+    </row>
+    <row r="29" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="22"/>
+    </row>
+    <row r="30" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="22"/>
+    </row>
+    <row r="31" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="22"/>
+    </row>
+    <row r="32" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="22"/>
+    </row>
+    <row r="33" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="22"/>
+    </row>
+    <row r="34" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="22"/>
+    </row>
+    <row r="35" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="22"/>
+    </row>
+    <row r="36" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="22"/>
+    </row>
+    <row r="37" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="28"/>
+    </row>
+    <row r="38" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="28"/>
+    </row>
+    <row r="39" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="28"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="29"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="27"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="8"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="27"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="28"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="8"/>
+      <c r="H44" s="28"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="27"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="21"/>
+    </row>
+  </sheetData>
+  <dataConsolidate>
+    <dataRefs count="1">
+      <dataRef ref="A2:H2" sheet="Status" r:id="rId1"/>
+    </dataRefs>
+  </dataConsolidate>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{738D911E-0DE6-44CE-B67D-4BFD958ECD8C}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -4378,7 +5217,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -4436,7 +5275,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
@@ -4451,30 +5290,30 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4743,421 +5582,6 @@
       <c r="B45" s="27"/>
       <c r="D45" s="4"/>
       <c r="E45" s="56"/>
-    </row>
-  </sheetData>
-  <dataConsolidate>
-    <dataRefs count="1">
-      <dataRef ref="A2:H2" sheet="Status" r:id="rId1"/>
-    </dataRefs>
-  </dataConsolidate>
-  <mergeCells count="3">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B0327C-9953-4813-9573-3D0583D807FE}">
-  <sheetPr>
-    <tabColor theme="0"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:H47"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="46.5703125" style="33" customWidth="1"/>
-    <col min="6" max="6" width="99.7109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="41.42578125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-    </row>
-    <row r="2" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-    </row>
-    <row r="3" spans="1:7" s="55" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-    </row>
-    <row r="4" spans="1:7" s="11" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="54" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="53"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="39" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" s="39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8" s="39" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="40" t="s">
-        <v>144</v>
-      </c>
-      <c r="F9" s="39" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="14" spans="1:7" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="28"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="28"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="28"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="28"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="27"/>
-      <c r="D18" s="4"/>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="D19" s="4"/>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="D21" s="4"/>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="55"/>
-    </row>
-    <row r="24" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="22"/>
-    </row>
-    <row r="25" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="22"/>
-    </row>
-    <row r="26" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="22"/>
-    </row>
-    <row r="27" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="22"/>
-    </row>
-    <row r="28" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="22"/>
-    </row>
-    <row r="29" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="22"/>
-    </row>
-    <row r="30" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="28"/>
-      <c r="H30" s="22"/>
-    </row>
-    <row r="31" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="22"/>
-    </row>
-    <row r="32" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="22"/>
-    </row>
-    <row r="33" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="22"/>
-    </row>
-    <row r="34" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="22"/>
-    </row>
-    <row r="35" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="22"/>
-    </row>
-    <row r="36" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="22"/>
-    </row>
-    <row r="37" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="22"/>
-    </row>
-    <row r="38" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="22"/>
-    </row>
-    <row r="39" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="22"/>
-    </row>
-    <row r="40" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="28"/>
-    </row>
-    <row r="41" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="28"/>
-    </row>
-    <row r="42" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="28"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="27"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="29"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="27"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="8"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="28"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="27"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="8"/>
-      <c r="H47" s="28"/>
     </row>
   </sheetData>
   <dataConsolidate>

</xml_diff>